<commit_message>
Stats notebook for n agents data
</commit_message>
<xml_diff>
--- a/experiment_data/n_agents_data/agents_data.xlsx
+++ b/experiment_data/n_agents_data/agents_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miche\OneDrive\Desktop\Codenames Progetto PDE\Codenames-LLM\experiment_data\n_agents_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E278A9BC-9F36-4088-94EC-0587A35A2F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E8200B0-99FE-4113-95EC-43EE91589801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -468,13 +468,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">

</xml_diff>